<commit_message>
1) Synchronizing some of the reference designators on the BOM vs the schematic (capacitors specifically) 2) Removing the 50pos connector from the BOM -- its supposed to be 64 ... dumbass.
</commit_message>
<xml_diff>
--- a/Hardware/LAB-DEB429A/docs/LAB-DEB429A-BOM.xlsx
+++ b/Hardware/LAB-DEB429A/docs/LAB-DEB429A-BOM.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="0" windowWidth="10470" windowHeight="7200"/>
+    <workbookView xWindow="4800" yWindow="0" windowWidth="10470" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="330">
   <si>
     <t>BILL OF MATERIALS</t>
   </si>
@@ -113,12 +114,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>ESQ-125-13-G-D</t>
-  </si>
-  <si>
-    <t>CONN RCPT 50POS .100" DUAL GOLD</t>
-  </si>
-  <si>
     <t>ESP-12</t>
   </si>
   <si>
@@ -131,9 +126,6 @@
     <t>R7</t>
   </si>
   <si>
-    <t>C15</t>
-  </si>
-  <si>
     <t>SO-08M</t>
   </si>
   <si>
@@ -296,12 +288,6 @@
     <t>R5, R6</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C5, C11, C12, C16, C19, C20, C21, C22</t>
-  </si>
-  <si>
-    <t>C6, C7, C8, C9, C10, C13, C14, C17, C18</t>
-  </si>
-  <si>
     <t>LAB-DEB429A-Rev0 PCB</t>
   </si>
   <si>
@@ -494,9 +480,6 @@
     <t>Total Board Cost:</t>
   </si>
   <si>
-    <t>SAM8769-ND</t>
-  </si>
-  <si>
     <t>1276-4766-1-ND</t>
   </si>
   <si>
@@ -540,6 +523,498 @@
   </si>
   <si>
     <t>Reference Des. Not Marked</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>Partlist</t>
+  </si>
+  <si>
+    <t>exported</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>C:/Users/drmoore/Documents/PEGMA/Hardware/LAB-DEB429A/cad/LAB-DEB429.sch</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Parts</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>MPN</t>
+  </si>
+  <si>
+    <t>OC_FARNELL</t>
+  </si>
+  <si>
+    <t>OC_NEWARK</t>
+  </si>
+  <si>
+    <t>TP_SIGNAL_NAME</t>
+  </si>
+  <si>
+    <t>LEDCHIPLED_1206</t>
+  </si>
+  <si>
+    <t>CHIPLED_1206</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>R-US_0204/7</t>
+  </si>
+  <si>
+    <t>0204/7</t>
+  </si>
+  <si>
+    <t>R10,</t>
+  </si>
+  <si>
+    <t>R15,</t>
+  </si>
+  <si>
+    <t>R16,</t>
+  </si>
+  <si>
+    <t>R17,</t>
+  </si>
+  <si>
+    <t>R18,</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>RESISTOR,</t>
+  </si>
+  <si>
+    <t>American</t>
+  </si>
+  <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>C-USC0603</t>
+  </si>
+  <si>
+    <t>C0603</t>
+  </si>
+  <si>
+    <t>C1,</t>
+  </si>
+  <si>
+    <t>C2,</t>
+  </si>
+  <si>
+    <t>C3,</t>
+  </si>
+  <si>
+    <t>C4,</t>
+  </si>
+  <si>
+    <t>C5,</t>
+  </si>
+  <si>
+    <t>C6,</t>
+  </si>
+  <si>
+    <t>C7,</t>
+  </si>
+  <si>
+    <t>C8,</t>
+  </si>
+  <si>
+    <t>C9,</t>
+  </si>
+  <si>
+    <t>C10,</t>
+  </si>
+  <si>
+    <t>C11,</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>CAPACITOR,</t>
+  </si>
+  <si>
+    <t>0.22u</t>
+  </si>
+  <si>
+    <t>0R1</t>
+  </si>
+  <si>
+    <t>R-US_R0603</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>R8,</t>
+  </si>
+  <si>
+    <t>R9,</t>
+  </si>
+  <si>
+    <t>R11,</t>
+  </si>
+  <si>
+    <t>R12,</t>
+  </si>
+  <si>
+    <t>R13,</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>C13,</t>
+  </si>
+  <si>
+    <t>C14,</t>
+  </si>
+  <si>
+    <t>C15,</t>
+  </si>
+  <si>
+    <t>C16,</t>
+  </si>
+  <si>
+    <t>C17,</t>
+  </si>
+  <si>
+    <t>C18,</t>
+  </si>
+  <si>
+    <t>C19,</t>
+  </si>
+  <si>
+    <t>C20,</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>18.4K</t>
+  </si>
+  <si>
+    <t>2.2K</t>
+  </si>
+  <si>
+    <t>R5,</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>25AA512</t>
+  </si>
+  <si>
+    <t>25MPX</t>
+  </si>
+  <si>
+    <t>39K</t>
+  </si>
+  <si>
+    <t>51K</t>
+  </si>
+  <si>
+    <t>HIH6131</t>
+  </si>
+  <si>
+    <t>LAB-ASDM300F</t>
+  </si>
+  <si>
+    <t>U1,</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U22,</t>
+  </si>
+  <si>
+    <t>U23,</t>
+  </si>
+  <si>
+    <t>U24</t>
+  </si>
+  <si>
+    <t>U4,</t>
+  </si>
+  <si>
+    <t>U5,</t>
+  </si>
+  <si>
+    <t>U6,</t>
+  </si>
+  <si>
+    <t>U12,</t>
+  </si>
+  <si>
+    <t>U13,</t>
+  </si>
+  <si>
+    <t>U14,</t>
+  </si>
+  <si>
+    <t>U16,</t>
+  </si>
+  <si>
+    <t>U18</t>
+  </si>
+  <si>
+    <t>LTC6244</t>
+  </si>
+  <si>
+    <t>U3,</t>
+  </si>
+  <si>
+    <t>U21</t>
+  </si>
+  <si>
+    <t>Low-noise,</t>
+  </si>
+  <si>
+    <t>high-speed</t>
+  </si>
+  <si>
+    <t>rail-to-rail</t>
+  </si>
+  <si>
+    <t>CMOS</t>
+  </si>
+  <si>
+    <t>op-amp</t>
+  </si>
+  <si>
+    <t>MAX4376HAUK</t>
+  </si>
+  <si>
+    <t>MAX4376</t>
+  </si>
+  <si>
+    <t>MM74HC259MTCX</t>
+  </si>
+  <si>
+    <t>SOP65P640X90-16N</t>
+  </si>
+  <si>
+    <t>U19,</t>
+  </si>
+  <si>
+    <t>U20</t>
+  </si>
+  <si>
+    <t>8-Bit</t>
+  </si>
+  <si>
+    <t>Addressable</t>
+  </si>
+  <si>
+    <t>Latch/3-to-8</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>Decoder</t>
+  </si>
+  <si>
+    <t>58K1947</t>
+  </si>
+  <si>
+    <t>FAIRCHILD</t>
+  </si>
+  <si>
+    <t>SEMICONDUCTOR</t>
+  </si>
+  <si>
+    <t>MICROSD</t>
+  </si>
+  <si>
+    <t>SI1143</t>
+  </si>
+  <si>
+    <t>SPBT2632C1A</t>
+  </si>
+  <si>
+    <t>SST26VF</t>
+  </si>
+  <si>
+    <t>TPPAD1-13</t>
+  </si>
+  <si>
+    <t>P1-13</t>
+  </si>
+  <si>
+    <t>TP1,</t>
+  </si>
+  <si>
+    <t>TP2,</t>
+  </si>
+  <si>
+    <t>TP3,</t>
+  </si>
+  <si>
+    <t>TP4,</t>
+  </si>
+  <si>
+    <t>TP5,</t>
+  </si>
+  <si>
+    <t>TP6,</t>
+  </si>
+  <si>
+    <t>TP7,</t>
+  </si>
+  <si>
+    <t>TP8,</t>
+  </si>
+  <si>
+    <t>TP9,</t>
+  </si>
+  <si>
+    <t>TP10,</t>
+  </si>
+  <si>
+    <t>TP11,</t>
+  </si>
+  <si>
+    <t>TP12,</t>
+  </si>
+  <si>
+    <t>TP13,</t>
+  </si>
+  <si>
+    <t>TP14,</t>
+  </si>
+  <si>
+    <t>TP15,</t>
+  </si>
+  <si>
+    <t>TP16,</t>
+  </si>
+  <si>
+    <t>TP17,</t>
+  </si>
+  <si>
+    <t>TP18,</t>
+  </si>
+  <si>
+    <t>TP19,</t>
+  </si>
+  <si>
+    <t>TP20,</t>
+  </si>
+  <si>
+    <t>TP21,</t>
+  </si>
+  <si>
+    <t>TP22,</t>
+  </si>
+  <si>
+    <t>TP23,</t>
+  </si>
+  <si>
+    <t>TP24,</t>
+  </si>
+  <si>
+    <t>TP25,</t>
+  </si>
+  <si>
+    <t>TP26,</t>
+  </si>
+  <si>
+    <t>TP27,</t>
+  </si>
+  <si>
+    <t>TP28,</t>
+  </si>
+  <si>
+    <t>TP29,</t>
+  </si>
+  <si>
+    <t>TP30,</t>
+  </si>
+  <si>
+    <t>TP31</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>pad</t>
+  </si>
+  <si>
+    <t>TSW-132-02-S-D</t>
+  </si>
+  <si>
+    <t>J1,</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>THROUGH-HOLE</t>
+  </si>
+  <si>
+    <t>.025"</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>HEADER</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>C13, C14, C15, C16, C17, C18, C19, C20, C22</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C12</t>
+  </si>
+  <si>
+    <t>64 POS, INSPECT HEIGHT</t>
   </si>
 </sst>
 </file>
@@ -742,7 +1217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -802,6 +1277,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -823,13 +1305,8 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1114,7 +1591,7 @@
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,11 +1621,11 @@
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="27"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
@@ -1159,10 +1636,10 @@
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="29"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
       <c r="G3" s="2"/>
@@ -1173,10 +1650,10 @@
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="2"/>
@@ -1187,10 +1664,10 @@
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
       <c r="G5" s="2"/>
@@ -1201,10 +1678,10 @@
       <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="31"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
       <c r="G6" s="2"/>
@@ -1252,10 +1729,10 @@
         <v>13</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1263,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>14</v>
@@ -1289,20 +1766,20 @@
       <c r="A10" s="10">
         <v>2</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>134</v>
+      <c r="B10" s="25" t="s">
+        <v>129</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -1311,7 +1788,7 @@
         <v>16</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="K10">
         <v>25.54</v>
@@ -1325,66 +1802,52 @@
       <c r="A11" s="10">
         <v>3</v>
       </c>
-      <c r="B11" s="22" t="s">
-        <v>29</v>
-      </c>
+      <c r="B11" s="22"/>
       <c r="C11" s="11"/>
       <c r="D11" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>74</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="E11" s="11"/>
       <c r="F11" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G11" s="11">
         <v>2</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="K11" s="23">
-        <v>6.9173999999999998</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="0"/>
-        <v>13.8348</v>
-      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="E12" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G12" s="11">
         <v>2</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K12" s="23">
         <v>0</v>
@@ -1399,31 +1862,31 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G13" s="11">
         <v>8</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K13" s="23">
         <v>0</v>
@@ -1438,31 +1901,31 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G14" s="11">
         <v>3</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K14" s="23">
         <v>0</v>
@@ -1476,20 +1939,20 @@
       <c r="A15" s="10">
         <v>7</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>98</v>
+      <c r="B15" s="25" t="s">
+        <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G15" s="11">
         <v>2</v>
@@ -1498,7 +1961,7 @@
         <v>16</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="K15" s="23">
         <v>2.35</v>
@@ -1512,20 +1975,20 @@
       <c r="A16" s="10">
         <v>8</v>
       </c>
-      <c r="B16" s="32" t="s">
-        <v>100</v>
+      <c r="B16" s="25" t="s">
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G16" s="11">
         <v>1</v>
@@ -1534,7 +1997,7 @@
         <v>16</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K16" s="23">
         <v>2.3210000000000002</v>
@@ -1549,19 +2012,19 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G17" s="11">
         <v>1</v>
@@ -1570,7 +2033,7 @@
         <v>16</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="K17" s="23">
         <v>10.057</v>
@@ -1585,19 +2048,19 @@
         <v>10</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G18" s="11">
         <v>1</v>
@@ -1606,7 +2069,7 @@
         <v>16</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="K18" s="23">
         <v>1.7</v>
@@ -1620,20 +2083,20 @@
       <c r="A19" s="10">
         <v>11</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="26">
         <v>5008730806</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G19" s="11">
         <v>1</v>
@@ -1643,7 +2106,7 @@
         <v>16</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K19" s="23">
         <v>3.802</v>
@@ -1657,20 +2120,20 @@
       <c r="A20" s="10">
         <v>12</v>
       </c>
-      <c r="B20" s="32" t="s">
-        <v>109</v>
+      <c r="B20" s="25" t="s">
+        <v>104</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G20" s="11">
         <v>1</v>
@@ -1679,7 +2142,7 @@
         <v>16</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K20" s="23">
         <v>0.78100000000000003</v>
@@ -1693,20 +2156,20 @@
       <c r="A21" s="10">
         <v>13</v>
       </c>
-      <c r="B21" s="32" t="s">
-        <v>111</v>
+      <c r="B21" s="25" t="s">
+        <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G21" s="11">
         <v>1</v>
@@ -1715,7 +2178,7 @@
         <v>16</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K21" s="23">
         <v>4.38</v>
@@ -1729,20 +2192,20 @@
       <c r="A22" s="10">
         <v>14</v>
       </c>
-      <c r="B22" s="32" t="s">
-        <v>116</v>
+      <c r="B22" s="25" t="s">
+        <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G22" s="11">
         <v>1</v>
@@ -1751,7 +2214,7 @@
         <v>16</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K22" s="23">
         <v>1.1599999999999999</v>
@@ -1765,20 +2228,20 @@
       <c r="A23" s="10">
         <v>15</v>
       </c>
-      <c r="B23" s="32" t="s">
-        <v>118</v>
+      <c r="B23" s="25" t="s">
+        <v>113</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G23" s="11">
         <v>2</v>
@@ -1787,7 +2250,7 @@
         <v>16</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K23" s="23">
         <v>0.46400000000000002</v>
@@ -1802,28 +2265,28 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G24" s="11">
         <v>1</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="K24" s="23">
         <v>6.26</v>
@@ -1837,20 +2300,20 @@
       <c r="A25" s="10">
         <v>17</v>
       </c>
-      <c r="B25" s="32" t="s">
-        <v>124</v>
+      <c r="B25" s="25" t="s">
+        <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G25" s="11">
         <v>1</v>
@@ -1859,7 +2322,7 @@
         <v>16</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K25" s="23">
         <v>20.393999999999998</v>
@@ -1874,19 +2337,19 @@
         <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G26" s="11">
         <v>1</v>
@@ -1895,7 +2358,7 @@
         <v>16</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="K26" s="23">
         <v>18.728999999999999</v>
@@ -1909,20 +2372,20 @@
       <c r="A27" s="10">
         <v>19</v>
       </c>
-      <c r="B27" s="32" t="s">
-        <v>129</v>
+      <c r="B27" s="25" t="s">
+        <v>124</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G27" s="10">
         <v>1</v>
@@ -1932,7 +2395,7 @@
         <v>16</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="K27" s="23">
         <v>0.13952000000000001</v>
@@ -1946,20 +2409,20 @@
       <c r="A28" s="10">
         <v>20</v>
       </c>
-      <c r="B28" s="32" t="s">
-        <v>142</v>
+      <c r="B28" s="25" t="s">
+        <v>137</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G28" s="10">
         <v>1</v>
@@ -1969,7 +2432,7 @@
         <v>16</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="K28" s="23">
         <v>1.4E-2</v>
@@ -1983,20 +2446,20 @@
       <c r="A29" s="10">
         <v>21</v>
       </c>
-      <c r="B29" s="32" t="s">
-        <v>144</v>
+      <c r="B29" s="25" t="s">
+        <v>139</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G29" s="10">
         <v>1</v>
@@ -2006,7 +2469,7 @@
         <v>16</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="K29" s="23">
         <v>1.4E-2</v>
@@ -2020,20 +2483,20 @@
       <c r="A30" s="10">
         <v>22</v>
       </c>
-      <c r="B30" s="32" t="s">
-        <v>159</v>
+      <c r="B30" s="25" t="s">
+        <v>153</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G30" s="10">
         <v>1</v>
@@ -2043,7 +2506,7 @@
         <v>16</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K30" s="23">
         <v>1.4E-2</v>
@@ -2057,20 +2520,20 @@
       <c r="A31" s="10">
         <v>23</v>
       </c>
-      <c r="B31" s="32" t="s">
-        <v>148</v>
+      <c r="B31" s="25" t="s">
+        <v>143</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G31" s="10">
         <v>1</v>
@@ -2080,7 +2543,7 @@
         <v>16</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="K31" s="23">
         <v>1.4E-2</v>
@@ -2094,20 +2557,20 @@
       <c r="A32" s="10">
         <v>24</v>
       </c>
-      <c r="B32" s="32" t="s">
-        <v>151</v>
+      <c r="B32" s="25" t="s">
+        <v>146</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G32" s="17">
         <v>1</v>
@@ -2117,7 +2580,7 @@
         <v>16</v>
       </c>
       <c r="J32" s="14" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K32" s="23">
         <v>3.48E-3</v>
@@ -2132,19 +2595,19 @@
         <v>25</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>18</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G33" s="10">
         <v>1</v>
@@ -2154,7 +2617,7 @@
         <v>16</v>
       </c>
       <c r="J33" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="K33" s="23">
         <v>3.4320000000000003E-2</v>
@@ -2168,20 +2631,20 @@
       <c r="A34" s="10">
         <v>26</v>
       </c>
-      <c r="B34" s="32" t="s">
-        <v>140</v>
+      <c r="B34" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E34" t="s">
         <v>20</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G34" s="10">
         <v>6</v>
@@ -2191,7 +2654,7 @@
         <v>16</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K34" s="23">
         <v>5.7000000000000002E-3</v>
@@ -2201,7 +2664,7 @@
         <v>3.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>27</v>
       </c>
@@ -2217,8 +2680,8 @@
       <c r="E35" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="20" t="s">
-        <v>90</v>
+      <c r="F35" s="10" t="s">
+        <v>328</v>
       </c>
       <c r="G35" s="10">
         <v>12</v>
@@ -2242,20 +2705,20 @@
       <c r="A36" s="10">
         <v>28</v>
       </c>
-      <c r="B36" s="32" t="s">
-        <v>137</v>
+      <c r="B36" s="25" t="s">
+        <v>132</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="G36" s="10">
         <v>1</v>
@@ -2265,7 +2728,7 @@
         <v>16</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K36" s="23">
         <v>3.5000000000000003E-2</v>
@@ -2292,10 +2755,10 @@
         <v>20</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>91</v>
+        <v>327</v>
       </c>
       <c r="G37" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H37"/>
       <c r="I37" s="10" t="s">
@@ -2309,27 +2772,27 @@
       </c>
       <c r="L37">
         <f t="shared" si="0"/>
-        <v>0.31553999999999999</v>
+        <v>0.35060000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>30</v>
       </c>
-      <c r="B38" s="32" t="s">
-        <v>161</v>
+      <c r="B38" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G38" s="10">
         <v>6</v>
@@ -2338,7 +2801,7 @@
         <v>16</v>
       </c>
       <c r="J38" s="14" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="K38" s="23">
         <v>5.8400000000000001E-2</v>
@@ -2352,32 +2815,32 @@
       <c r="A39" s="10">
         <v>31</v>
       </c>
-      <c r="B39" s="32" t="s">
-        <v>167</v>
+      <c r="B39" s="25" t="s">
+        <v>161</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G39" s="10">
         <v>13</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I39" s="10" t="s">
         <v>16</v>
       </c>
       <c r="J39" s="14" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="K39" s="23">
         <v>0.08</v>
@@ -2388,12 +2851,12 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K40" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="L40" s="34">
+      <c r="K40" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="L40" s="27">
         <f>SUM(L9:L39)</f>
-        <v>127.28437999999997</v>
+        <v>113.48463999999997</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2448,12 +2911,973 @@
     <hyperlink ref="J29" r:id="rId24" display="http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/RC1608F393CS/1276-4798-1-ND/3967770"/>
     <hyperlink ref="J31" r:id="rId25" display="http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/RC1608F300CS/1276-4521-1-ND/3967493"/>
     <hyperlink ref="J32" r:id="rId26" display="http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/RC1608F102CS/1276-3484-1-ND/3903587"/>
-    <hyperlink ref="J11" r:id="rId27" display="http://www.digikey.com/product-detail/en/samtec-inc/ESQ-125-13-G-D/SAM8769-ND/2640984"/>
-    <hyperlink ref="J30" r:id="rId28" display="http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/RC1608F1822CS/1276-4766-1-ND/3967738"/>
-    <hyperlink ref="J38" r:id="rId29" display="http://www.digikey.com/product-detail/en/yageo/FMP100JR-52-3R3/3.3WCT-ND/2058924"/>
-    <hyperlink ref="J39" r:id="rId30" display="http://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/1-2199298-2/A120347-ND/5022039"/>
+    <hyperlink ref="J30" r:id="rId27" display="http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/RC1608F1822CS/1276-4766-1-ND/3967738"/>
+    <hyperlink ref="J38" r:id="rId28" display="http://www.digikey.com/product-detail/en/yageo/FMP100JR-52-3R3/3.3WCT-ND/2058924"/>
+    <hyperlink ref="J39" r:id="rId29" display="http://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/1-2199298-2/A120347-ND/5022039"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="35">
+        <v>42480</v>
+      </c>
+      <c r="G1" s="36">
+        <v>0.33606481481481482</v>
+      </c>
+      <c r="H1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J3" t="s">
+        <v>182</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6" t="s">
+        <v>191</v>
+      </c>
+      <c r="G6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" t="s">
+        <v>193</v>
+      </c>
+      <c r="I6" t="s">
+        <v>194</v>
+      </c>
+      <c r="J6" t="s">
+        <v>195</v>
+      </c>
+      <c r="K6" t="s">
+        <v>196</v>
+      </c>
+      <c r="L6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H7" t="s">
+        <v>204</v>
+      </c>
+      <c r="I7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K7" t="s">
+        <v>207</v>
+      </c>
+      <c r="L7" t="s">
+        <v>208</v>
+      </c>
+      <c r="M7" t="s">
+        <v>209</v>
+      </c>
+      <c r="N7" t="s">
+        <v>210</v>
+      </c>
+      <c r="O7" t="s">
+        <v>211</v>
+      </c>
+      <c r="P7" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>213</v>
+      </c>
+      <c r="R7" t="s">
+        <v>196</v>
+      </c>
+      <c r="S7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" t="s">
+        <v>213</v>
+      </c>
+      <c r="G8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" t="s">
+        <v>219</v>
+      </c>
+      <c r="G10" t="s">
+        <v>220</v>
+      </c>
+      <c r="H10" t="s">
+        <v>221</v>
+      </c>
+      <c r="I10" t="s">
+        <v>222</v>
+      </c>
+      <c r="J10" t="s">
+        <v>223</v>
+      </c>
+      <c r="K10" t="s">
+        <v>195</v>
+      </c>
+      <c r="L10" t="s">
+        <v>196</v>
+      </c>
+      <c r="M10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" t="s">
+        <v>225</v>
+      </c>
+      <c r="F11" t="s">
+        <v>226</v>
+      </c>
+      <c r="G11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H11" t="s">
+        <v>228</v>
+      </c>
+      <c r="I11" t="s">
+        <v>229</v>
+      </c>
+      <c r="J11" t="s">
+        <v>230</v>
+      </c>
+      <c r="K11" t="s">
+        <v>231</v>
+      </c>
+      <c r="L11" t="s">
+        <v>232</v>
+      </c>
+      <c r="M11" t="s">
+        <v>233</v>
+      </c>
+      <c r="N11" t="s">
+        <v>213</v>
+      </c>
+      <c r="O11" t="s">
+        <v>196</v>
+      </c>
+      <c r="P11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>195</v>
+      </c>
+      <c r="G12" t="s">
+        <v>196</v>
+      </c>
+      <c r="H12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" t="s">
+        <v>216</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" t="s">
+        <v>237</v>
+      </c>
+      <c r="G13" t="s">
+        <v>195</v>
+      </c>
+      <c r="H13" t="s">
+        <v>196</v>
+      </c>
+      <c r="I13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" t="s">
+        <v>239</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G16" t="s">
+        <v>196</v>
+      </c>
+      <c r="H16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>240</v>
+      </c>
+      <c r="C17" t="s">
+        <v>216</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" t="s">
+        <v>195</v>
+      </c>
+      <c r="G17" t="s">
+        <v>196</v>
+      </c>
+      <c r="H17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>241</v>
+      </c>
+      <c r="C18" t="s">
+        <v>216</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>195</v>
+      </c>
+      <c r="G18" t="s">
+        <v>196</v>
+      </c>
+      <c r="H18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>242</v>
+      </c>
+      <c r="C19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>243</v>
+      </c>
+      <c r="E20" t="s">
+        <v>244</v>
+      </c>
+      <c r="F20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>246</v>
+      </c>
+      <c r="F21" t="s">
+        <v>247</v>
+      </c>
+      <c r="G21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>249</v>
+      </c>
+      <c r="F22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G22" t="s">
+        <v>251</v>
+      </c>
+      <c r="H22" t="s">
+        <v>252</v>
+      </c>
+      <c r="I22" t="s">
+        <v>253</v>
+      </c>
+      <c r="J22" t="s">
+        <v>254</v>
+      </c>
+      <c r="K22" t="s">
+        <v>255</v>
+      </c>
+      <c r="L22" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>257</v>
+      </c>
+      <c r="C23" t="s">
+        <v>257</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>258</v>
+      </c>
+      <c r="F23" t="s">
+        <v>259</v>
+      </c>
+      <c r="G23" t="s">
+        <v>260</v>
+      </c>
+      <c r="H23" t="s">
+        <v>261</v>
+      </c>
+      <c r="I23" t="s">
+        <v>262</v>
+      </c>
+      <c r="J23" t="s">
+        <v>263</v>
+      </c>
+      <c r="K23" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>265</v>
+      </c>
+      <c r="C24" t="s">
+        <v>266</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>267</v>
+      </c>
+      <c r="C25" t="s">
+        <v>267</v>
+      </c>
+      <c r="D25" t="s">
+        <v>268</v>
+      </c>
+      <c r="E25" t="s">
+        <v>269</v>
+      </c>
+      <c r="F25" t="s">
+        <v>270</v>
+      </c>
+      <c r="G25" t="s">
+        <v>271</v>
+      </c>
+      <c r="H25" t="s">
+        <v>272</v>
+      </c>
+      <c r="I25" t="s">
+        <v>273</v>
+      </c>
+      <c r="J25" t="s">
+        <v>274</v>
+      </c>
+      <c r="K25" t="s">
+        <v>275</v>
+      </c>
+      <c r="L25" t="s">
+        <v>267</v>
+      </c>
+      <c r="M25">
+        <v>1607831</v>
+      </c>
+      <c r="N25" t="s">
+        <v>276</v>
+      </c>
+      <c r="O25" t="s">
+        <v>44</v>
+      </c>
+      <c r="P25" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>279</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C27" t="s">
+        <v>280</v>
+      </c>
+      <c r="D27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>281</v>
+      </c>
+      <c r="C28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D28" t="s">
+        <v>281</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>282</v>
+      </c>
+      <c r="C29" t="s">
+        <v>282</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C30" t="s">
+        <v>283</v>
+      </c>
+      <c r="D30" t="s">
+        <v>284</v>
+      </c>
+      <c r="E30" t="s">
+        <v>285</v>
+      </c>
+      <c r="F30" t="s">
+        <v>286</v>
+      </c>
+      <c r="G30" t="s">
+        <v>287</v>
+      </c>
+      <c r="H30" t="s">
+        <v>288</v>
+      </c>
+      <c r="I30" t="s">
+        <v>289</v>
+      </c>
+      <c r="J30" t="s">
+        <v>290</v>
+      </c>
+      <c r="K30" t="s">
+        <v>291</v>
+      </c>
+      <c r="L30" t="s">
+        <v>292</v>
+      </c>
+      <c r="M30" t="s">
+        <v>293</v>
+      </c>
+      <c r="N30" t="s">
+        <v>294</v>
+      </c>
+      <c r="O30" t="s">
+        <v>295</v>
+      </c>
+      <c r="P30" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>297</v>
+      </c>
+      <c r="R30" t="s">
+        <v>298</v>
+      </c>
+      <c r="S30" t="s">
+        <v>299</v>
+      </c>
+      <c r="T30" t="s">
+        <v>300</v>
+      </c>
+      <c r="U30" t="s">
+        <v>301</v>
+      </c>
+      <c r="V30" t="s">
+        <v>302</v>
+      </c>
+      <c r="W30" t="s">
+        <v>303</v>
+      </c>
+      <c r="X30" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>305</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>306</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>307</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>308</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>309</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>311</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>312</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>313</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>314</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>315</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>316</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>318</v>
+      </c>
+      <c r="C31" t="s">
+        <v>318</v>
+      </c>
+      <c r="D31" t="s">
+        <v>318</v>
+      </c>
+      <c r="E31" t="s">
+        <v>319</v>
+      </c>
+      <c r="F31" t="s">
+        <v>320</v>
+      </c>
+      <c r="G31" t="s">
+        <v>321</v>
+      </c>
+      <c r="H31" t="s">
+        <v>322</v>
+      </c>
+      <c r="I31" t="s">
+        <v>323</v>
+      </c>
+      <c r="J31" t="s">
+        <v>324</v>
+      </c>
+      <c r="K31" t="s">
+        <v>325</v>
+      </c>
+      <c r="L31" t="s">
+        <v>326</v>
+      </c>
+      <c r="M31" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1) Adding some notes to the schematic and bringing out some datasheets.
</commit_message>
<xml_diff>
--- a/Hardware/LAB-DEB429A/docs/LAB-DEB429A-BOM.xlsx
+++ b/Hardware/LAB-DEB429A/docs/LAB-DEB429A-BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="10470" windowHeight="7200"/>
+    <workbookView xWindow="7230" yWindow="0" windowWidth="10470" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="2" r:id="rId1"/>
@@ -1284,6 +1284,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1305,8 +1307,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1590,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="B20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,11 +1621,11 @@
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
@@ -1636,10 +1636,10 @@
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="32"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
       <c r="G3" s="2"/>
@@ -1650,10 +1650,10 @@
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="2"/>
@@ -1664,10 +1664,10 @@
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="32"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
       <c r="G5" s="2"/>
@@ -1678,10 +1678,10 @@
       <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
       <c r="G6" s="2"/>
@@ -2946,10 +2946,10 @@
       <c r="E1" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="35">
+      <c r="F1" s="28">
         <v>42480</v>
       </c>
-      <c r="G1" s="36">
+      <c r="G1" s="29">
         <v>0.33606481481481482</v>
       </c>
       <c r="H1" t="s">

</xml_diff>